<commit_message>
Minor edits made to configuration logs
</commit_message>
<xml_diff>
--- a/Configurations/CM_1.1.0_10032019.xlsx
+++ b/Configurations/CM_1.1.0_10032019.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ming Yu\Documents\SMU\IS214\transfer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ming Yu\Documents\SMU\IS214\esm214\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1662F434-1CF6-4B06-8885-601326292F5D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D06B32-1C32-41C6-B1B1-4CC9B5DB5E18}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{2BB56906-853E-4336-8E30-9BAFB26AF772}"/>
   </bookViews>
   <sheets>
-    <sheet name="SCP 1.0.5" sheetId="1" r:id="rId1"/>
+    <sheet name="SCP 1.1.0" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -709,7 +709,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>

</xml_diff>